<commit_message>
notebook 1 et 2
</commit_message>
<xml_diff>
--- a/human_rating/reviews_reproducibility_2023.xlsx
+++ b/human_rating/reviews_reproducibility_2023.xlsx
@@ -2128,7 +2128,11 @@
           <t>Authors have indicated that the code will be released upon acceptance. This in conjunction with the observation that the model is evaluated on public benchmark would significant help with reproducibility.</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -3015,7 +3019,11 @@
           <t>Method should not be difficult to reproduce. For the data, authors are using 9,544 MRIs from ADNI. However, it is unclear if they plan to release the tissue segmentation maps.</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
@@ -4703,7 +4711,11 @@
           <t>I believe that the obtained results can, in principle, be reproduced. Even though key resources (e.g., code) are unavailable at this point, the key details (e.g., proof sketches, experimental setup) are sufficiently well described for an expert to confidently reproduce the main results, if given access to the missing resources.</t>
         </is>
       </c>
-      <c r="D159" t="inlineStr"/>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
       <c r="E159" t="inlineStr">
         <is>
           <t>Reasonable.</t>
@@ -5320,7 +5332,11 @@
           <t>The authors meet all criteria on the reproducibility checklist But the pre-trained model</t>
         </is>
       </c>
-      <c r="D182" t="inlineStr"/>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
       <c r="E182" t="inlineStr">
         <is>
           <t>The code will be made available if accepted</t>
@@ -6094,7 +6110,11 @@
           <t>Discovering Brain Network Dysfunction in Alzheimer's Disease Using Brain Hypergraph Neural Network</t>
         </is>
       </c>
-      <c r="C211" t="inlineStr"/>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
       <c r="D211" t="inlineStr">
         <is>
           <t>The data is from a public dataset and the details for reproduction is provided.</t>
@@ -8206,7 +8226,11 @@
           <t>Seems reproducible.</t>
         </is>
       </c>
-      <c r="E289" t="inlineStr"/>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
@@ -12864,7 +12888,11 @@
           <t>The authors use an internal dataset. In the checklist, they select to provide the codes, data, and model. However, these informations do not appear in the paper.</t>
         </is>
       </c>
-      <c r="D462" t="inlineStr"/>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="E462" t="inlineStr">
         <is>
           <t>I believe that this paper has the potential to contribute to the community through its reproducibility, especially if the authors open-source their code and software. This would allow other researchers to easily replicate their results and build upon their findings.</t>
@@ -13131,7 +13159,11 @@
           <t>Should be okay if code is provided.</t>
         </is>
       </c>
-      <c r="E472" t="inlineStr"/>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="473">
       <c r="A473" s="1" t="inlineStr">
@@ -16561,7 +16593,11 @@
           <t>Shifting More Attention to Breast Lesion Segmentation in Ultrasound Videos</t>
         </is>
       </c>
-      <c r="C600" t="inlineStr"/>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="D600" t="inlineStr">
         <is>
           <t>The authors will release the dataset and model.</t>

</xml_diff>